<commit_message>
Manual commit [周一 2025/04/14 14:18:51.20]
</commit_message>
<xml_diff>
--- a/热电偶/工作簿1.xlsx
+++ b/热电偶/工作簿1.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhouzhou/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\30752\Desktop\guest\edit\热电偶\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6253E229-3186-DF45-9B66-314B6327B029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8701671C-E636-4043-A734-7A462ECAE5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10600" yWindow="6180" windowWidth="17840" windowHeight="11220" xr2:uid="{6EC8B40A-9E5B-7845-94F4-5FB6BC71BD45}"/>
+    <workbookView xWindow="4635" yWindow="2475" windowWidth="21600" windowHeight="12645" xr2:uid="{6EC8B40A-9E5B-7845-94F4-5FB6BC71BD45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,9 +36,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="0.000_ "/>
+    <numFmt numFmtId="176" formatCode="0.000_ "/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -154,7 +152,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -491,19 +489,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F402F9-9609-DD4B-9730-A53C077AF220}">
-  <dimension ref="A5:K10"/>
+  <dimension ref="A5:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:K10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="11" width="10.83203125" style="5"/>
+    <col min="9" max="11" width="10.875" style="5"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:11" ht="17" thickBot="1"/>
-    <row r="6" spans="1:11" ht="17" thickBot="1">
+    <row r="5" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>40</v>
       </c>
@@ -537,8 +535,20 @@
         <f>ABS(I6-A6)</f>
         <v>0.10000000000000142</v>
       </c>
+      <c r="M6">
+        <f>0.99892*I6-0.01476</f>
+        <v>40.041932000000003</v>
+      </c>
+      <c r="N6">
+        <f>ABS(M6-A6)</f>
+        <v>4.1932000000002745E-2</v>
+      </c>
+      <c r="O6">
+        <f>N6/A6</f>
+        <v>1.0483000000000686E-3</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" ht="17" thickBot="1">
+    <row r="7" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45.06</v>
       </c>
@@ -572,8 +582,20 @@
         <f t="shared" ref="K7:K10" si="2">ABS(I7-A7)</f>
         <v>0.11000000000000654</v>
       </c>
+      <c r="M7">
+        <f t="shared" ref="M7:M10" si="3">0.99892*I7-0.01476</f>
+        <v>44.886693999999991</v>
+      </c>
+      <c r="N7">
+        <f t="shared" ref="N7:N10" si="4">ABS(M7-A7)</f>
+        <v>0.17330600000001084</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ref="O7:O10" si="5">N7/A7</f>
+        <v>3.8461162893921623E-3</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" ht="17" thickBot="1">
+    <row r="8" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>49.96</v>
       </c>
@@ -607,8 +629,20 @@
         <f t="shared" si="2"/>
         <v>0.29333333333332945</v>
       </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>50.184299733333326</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>0.22429973333332498</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="5"/>
+        <v>4.4895863357350876E-3</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" ht="17" thickBot="1">
+    <row r="9" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>55.01</v>
       </c>
@@ -642,8 +676,20 @@
         <f t="shared" si="2"/>
         <v>9.9999999999980105E-3</v>
       </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>54.925840000000001</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>8.4159999999997126E-2</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="5"/>
+        <v>1.5299036538810604E-3</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" ht="17" thickBot="1">
+    <row r="10" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>60</v>
       </c>
@@ -676,10 +722,33 @@
       <c r="K10" s="5">
         <f t="shared" si="2"/>
         <v>7.0000000000000284E-2</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>59.990364399999997</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>9.635600000002853E-3</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="5"/>
+        <v>1.6059333333338089E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <f>SUM(N6:N10)/5</f>
+        <v>0.10666666666666771</v>
+      </c>
+      <c r="O14">
+        <f>SUM(O6:O10)/5</f>
+        <v>2.2148999224683519E-3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>